<commit_message>
All tests complete - all tests succeed
</commit_message>
<xml_diff>
--- a/ClueLayout/Layout.xlsx
+++ b/ClueLayout/Layout.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="23940" windowHeight="11100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="21">
   <si>
     <t>X</t>
   </si>
@@ -445,15 +446,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -520,11 +521,14 @@
       <c r="V1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -591,11 +595,14 @@
       <c r="V2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -662,11 +669,14 @@
       <c r="V3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -733,11 +743,14 @@
       <c r="V4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -804,11 +817,14 @@
       <c r="V5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -875,11 +891,14 @@
       <c r="V6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -946,11 +965,14 @@
       <c r="V7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1017,11 +1039,14 @@
       <c r="V8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1088,11 +1113,14 @@
       <c r="V9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="X9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1159,11 +1187,14 @@
       <c r="V10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="W10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="X10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1230,11 +1261,14 @@
       <c r="V11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="X11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1301,11 +1335,14 @@
       <c r="V12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="X12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1372,11 +1409,14 @@
       <c r="V13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W13">
+      <c r="W13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1443,11 +1483,14 @@
       <c r="V14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W14">
+      <c r="W14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1514,11 +1557,14 @@
       <c r="V15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W15">
+      <c r="W15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1585,11 +1631,14 @@
       <c r="V16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="W16">
+      <c r="W16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1653,14 +1702,17 @@
       <c r="U17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="V17" s="4" t="s">
+      <c r="V17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -1727,11 +1779,14 @@
       <c r="V18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W18">
+      <c r="W18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1798,11 +1853,14 @@
       <c r="V19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W19">
+      <c r="W19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X19">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1869,11 +1927,14 @@
       <c r="V20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W20">
+      <c r="W20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X20">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -1940,11 +2001,14 @@
       <c r="V21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W21">
+      <c r="W21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -2011,11 +2075,14 @@
       <c r="V22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W22">
+      <c r="W22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X22">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2071,15 +2138,18 @@
         <v>17</v>
       </c>
       <c r="S23">
+        <v>18</v>
+      </c>
+      <c r="T23">
         <v>19</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <v>20</v>
       </c>
-      <c r="U23">
+      <c r="V23">
         <v>21</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added skeleton for CluePlayers pt 1
</commit_message>
<xml_diff>
--- a/ClueLayout/Layout.xlsx
+++ b/ClueLayout/Layout.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse_000\workspace\ClueGame\ClueLayout\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="23940" windowHeight="11100"/>
   </bookViews>
@@ -117,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +167,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -213,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -226,6 +227,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -291,7 +294,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,7 +329,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -538,7 +541,7 @@
   <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +571,7 @@
       <c r="H1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="12" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -1595,7 +1598,7 @@
       <c r="E15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G15" s="3" t="s">

</xml_diff>

<commit_message>
bug fixes and config format changes
</commit_message>
<xml_diff>
--- a/ClueLayout/Layout.xlsx
+++ b/ClueLayout/Layout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="23940" windowHeight="11100"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -102,8 +102,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,7 +326,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -361,7 +360,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -537,16 +535,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -620,7 +618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -694,7 +692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -768,7 +766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -842,7 +840,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -916,7 +914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -990,7 +988,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1064,7 +1062,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1138,7 +1136,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
@@ -1212,7 +1210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1286,7 +1284,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1360,7 +1358,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1434,7 +1432,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
@@ -1508,7 +1506,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1582,7 +1580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1656,7 +1654,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1730,7 +1728,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1804,7 +1802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -1878,7 +1876,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1952,7 +1950,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -2026,7 +2024,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -2100,7 +2098,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -2174,7 +2172,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24">
       <c r="A23">
         <v>0</v>
       </c>
@@ -2245,32 +2243,32 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24">
       <c r="A25" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24">
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24">
       <c r="A27" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24">
       <c r="A28" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24">
       <c r="A29" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24">
       <c r="A30" s="6" t="s">
         <v>26</v>
       </c>
@@ -2282,24 +2280,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>